<commit_message>
Fix a typo on the meta page for OAMR gas works
</commit_message>
<xml_diff>
--- a/data-raw/FixedOAMRGasWorks.xlsx
+++ b/data-raw/FixedOAMRGasWorks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/IEATools/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC55E2FF-CAEE-B242-BD14-CC25806750D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4030D80-786F-5E46-9BAF-6A5575DF5C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20900" yWindow="3100" windowWidth="28040" windowHeight="23400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5160" yWindow="500" windowWidth="28040" windowHeight="23400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Meta" sheetId="2" r:id="rId1"/>
@@ -72,9 +72,6 @@
     <t>Production</t>
   </si>
   <si>
-    <t>produce Charcoal without consuming any feedstock,</t>
-  </si>
-  <si>
     <t>so OAMR Gas works appear to have infinite energy efficiency.</t>
   </si>
   <si>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t>Gas works</t>
+  </si>
+  <si>
+    <t>produce Gas works gas without consuming any feedstock,</t>
   </si>
 </sst>
 </file>
@@ -1007,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1030,42 +1030,42 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
@@ -1075,6 +1075,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1206,7 +1207,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6">
         <v>0.78794540000000002</v>
@@ -1237,7 +1238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{363DDDCC-90F7-484F-964D-C2923D8FF80C}">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
@@ -1256,31 +1257,31 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>25</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>26</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>27</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>28</v>
-      </c>
-      <c r="I1" t="s">
-        <v>29</v>
       </c>
       <c r="J1">
         <v>1971</v>
@@ -1303,22 +1304,22 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>11</v>
@@ -1327,7 +1328,7 @@
         <v>5</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J2" s="2">
         <f>'OAMR Gw IEA WEB 2022'!D2 + (-Fixed!J3)</f>
@@ -1356,31 +1357,31 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="F3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J3" s="2">
         <f>-J4/'OAMR Gw IEA WEB 2022'!D6</f>
@@ -1409,31 +1410,31 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="F4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J4">
         <v>82.8</v>

</xml_diff>